<commit_message>
Updated Figures, Model Results
</commit_message>
<xml_diff>
--- a/DeepESN/results.xlsx
+++ b/DeepESN/results.xlsx
@@ -581,24 +581,24 @@
         <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>1.743626889032091</v>
+        <v>1.541175203748385</v>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>1.337691932450526</v>
+        <v>1.167852480108754</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9463205604832144</v>
+        <v>0.9580622735172457</v>
       </c>
       <c r="R2" t="n">
-        <v>3.248854367799965</v>
+        <v>3.232744463347607</v>
       </c>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="n">
-        <v>2.711962228939682</v>
+        <v>2.654117159539461</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8411448956345002</v>
+        <v>0.842716400745953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>